<commit_message>
Update lobbyist data. Couple model updates
</commit_message>
<xml_diff>
--- a/data/Cam_ContribExpenditureLobbyistType.xlsx
+++ b/data/Cam_ContribExpenditureLobbyistType.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet sheetId="1" r:id="rId1" name="Cam_ContribExpenditureLobbyistT"/>
   </sheets>
+  <definedNames>
+    <definedName name="Cam_ContribExpenditureLobbyistType">'Cam_ContribExpenditureLobbyistT'!$A$1:$C$10</definedName>
+  </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
@@ -23,32 +26,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -56,36 +33,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -96,80 +43,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD0D7E5"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD0D7E5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD0D7E5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD0D7E5"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD0D7E5"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD0D7E5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD0D7E5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD0D7E5"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD0D7E5"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD0D7E5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD0D7E5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD0D7E5"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyFill="1" applyProtection="1" applyAlignment="1" applyFont="1" xfId="0">
-      <alignment wrapText="0" vertical="center" horizontal="left"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
-      <alignment wrapText="0" vertical="center" horizontal="center"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
-      <alignment wrapText="0" vertical="center" horizontal="center"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
-      <alignment wrapText="1" vertical="center" horizontal="right"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
-      <alignment wrapText="1" vertical="center" horizontal="general"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,143 +350,138 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="true" min="1" max="1" width="14.0625"/>
-    <col customWidth="true" min="2" max="2" width="14.0625"/>
-    <col customWidth="true" min="3" max="3" width="14.0625"/>
-  </cols>
   <sheetData>
     <row outlineLevel="0" r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>ContribExpenditureLobbyistTypeId</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>ContribExpenditureLobbyistTypeGroupId</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>Meal and Beverage Expenses</t>
         </is>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="0">
         <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>Entertainment Expenses</t>
         </is>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="0">
         <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="4">
-      <c r="A4" s="4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>Gift Expenses</t>
         </is>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="0">
         <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>Other Expenses</t>
         </is>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="0">
         <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>Political Contribution</t>
         </is>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="0">
         <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>Candidate</t>
         </is>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="0">
         <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>Public Official</t>
         </is>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="0">
         <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="9">
-      <c r="A9" s="4">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>Support Ballot Issue</t>
         </is>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="0">
         <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="10">
-      <c r="A10" s="4">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>Oppose Ballot Issue</t>
         </is>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="0">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tidy up search a bit. Add new lobbyist data
</commit_message>
<xml_diff>
--- a/data/Cam_ContribExpenditureLobbyistType.xlsx
+++ b/data/Cam_ContribExpenditureLobbyistType.xlsx
@@ -8,9 +8,10 @@
   </bookViews>
   <sheets>
     <sheet sheetId="1" r:id="rId1" name="Cam_ContribExpenditureLobbyistT"/>
+    <sheet r:id="rId4" name="Cam_ContribExpenditureLobbyist1" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="Cam_ContribExpenditureLobbyistType">'Cam_ContribExpenditureLobbyistT'!$A$1:$C$10</definedName>
+    <definedName name="Cam_ContribExpenditureLobbyistType">'Cam_ContribExpenditureLobbyist1'!$A$1:$C$10</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -488,4 +489,153 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row outlineLevel="0" r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>ContribExpenditureLobbyistTypeId</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>ContribExpenditureLobbyistTypeGroupId</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Meal and Beverage Expenses</t>
+        </is>
+      </c>
+      <c r="C2" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Entertainment Expenses</t>
+        </is>
+      </c>
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Gift Expenses</t>
+        </is>
+      </c>
+      <c r="C4" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Other Expenses</t>
+        </is>
+      </c>
+      <c r="C5" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Political Contribution</t>
+        </is>
+      </c>
+      <c r="C6" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Candidate</t>
+        </is>
+      </c>
+      <c r="C7" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Public Official</t>
+        </is>
+      </c>
+      <c r="C8" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Support Ballot Issue</t>
+        </is>
+      </c>
+      <c r="C9" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>Oppose Ballot Issue</t>
+        </is>
+      </c>
+      <c r="C10" s="0">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update data import for Fall 2019 data
</commit_message>
<xml_diff>
--- a/data/Cam_ContribExpenditureLobbyistType.xlsx
+++ b/data/Cam_ContribExpenditureLobbyistType.xlsx
@@ -1,41 +1,118 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CFIS Reports\NMInDepth - Childress\2019_11_Nov\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Cam_ContribExpenditureLobbyistT"/>
+    <sheet name="NMInDepth_Cam_ContribExpenditur" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="Cam_ContribExpenditureLobbyistType">'Cam_ContribExpenditureLobbyistT'!$A$1:$C$10</definedName>
-  </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>ContribExpenditureLobbyistTypeId</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ContribExpenditureLobbyistTypeGroupId</t>
+  </si>
+  <si>
+    <t>Meal and Beverage Expenses</t>
+  </si>
+  <si>
+    <t>Entertainment Expenses</t>
+  </si>
+  <si>
+    <t>Gift Expenses</t>
+  </si>
+  <si>
+    <t>Other Expenses</t>
+  </si>
+  <si>
+    <t>Political Contribution</t>
+  </si>
+  <si>
+    <t>Candidate</t>
+  </si>
+  <si>
+    <t>Public Official</t>
+  </si>
+  <si>
+    <t>Support Ballot Issue</t>
+  </si>
+  <si>
+    <t>Oppose Ballot Issue</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -43,18 +120,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0D7E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0D7E5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0D7E5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0D7E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0D7E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0D7E5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0D7E5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0D7E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -101,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,9 +272,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -167,6 +307,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -342,146 +483,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row outlineLevel="0" r="1">
-      <c r="A1" s="0" t="inlineStr">
-        <is>
-          <t>ContribExpenditureLobbyistTypeId</t>
-        </is>
-      </c>
-      <c r="B1" s="0" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="C1" s="0" t="inlineStr">
-        <is>
-          <t>ContribExpenditureLobbyistTypeGroupId</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="2">
-      <c r="A2" s="0">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Meal and Beverage Expenses</t>
-        </is>
-      </c>
-      <c r="C2" s="0">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row outlineLevel="0" r="3">
-      <c r="A3" s="0">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Entertainment Expenses</t>
-        </is>
-      </c>
-      <c r="C3" s="0">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row outlineLevel="0" r="4">
-      <c r="A4" s="0">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>Gift Expenses</t>
-        </is>
-      </c>
-      <c r="C4" s="0">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row outlineLevel="0" r="5">
-      <c r="A5" s="0">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>Other Expenses</t>
-        </is>
-      </c>
-      <c r="C5" s="0">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="0">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>Political Contribution</t>
-        </is>
-      </c>
-      <c r="C6" s="0">
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
         <v>2</v>
       </c>
     </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="0">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>Candidate</t>
-        </is>
-      </c>
-      <c r="C7" s="0">
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2">
         <v>2</v>
       </c>
     </row>
-    <row outlineLevel="0" r="8">
-      <c r="A8" s="0">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>Public Official</t>
-        </is>
-      </c>
-      <c r="C8" s="0">
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2">
         <v>2</v>
       </c>
     </row>
-    <row outlineLevel="0" r="9">
-      <c r="A9" s="0">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>Support Ballot Issue</t>
-        </is>
-      </c>
-      <c r="C9" s="0">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2">
         <v>2</v>
       </c>
     </row>
-    <row outlineLevel="0" r="10">
-      <c r="A10" s="0">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="inlineStr">
-        <is>
-          <t>Oppose Ballot Issue</t>
-        </is>
-      </c>
-      <c r="C10" s="0">
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data and import_data for Fall 2019 dump
</commit_message>
<xml_diff>
--- a/data/Cam_ContribExpenditureLobbyistType.xlsx
+++ b/data/Cam_ContribExpenditureLobbyistType.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Cam_ContribExpenditureLobbyistT"/>
+    <sheet sheetId="1" r:id="rId1" name="NMInDepth_Cam_ContribExpenditur"/>
   </sheets>
   <definedNames>
-    <definedName name="Cam_ContribExpenditureLobbyistType">'Cam_ContribExpenditureLobbyistT'!$A$1:$C$10</definedName>
+    <definedName name="NMInDepth_Cam_ContribExpenditureLobbyistType">'NMInDepth_Cam_ContribExpenditur'!$A$1:$C$10</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>

</xml_diff>